<commit_message>
subo algunas modificaciones - si hay algo mal SOY DARIO
</commit_message>
<xml_diff>
--- a/web/uploads/horarios informartica.xlsx
+++ b/web/uploads/horarios informartica.xlsx
@@ -43,9 +43,6 @@
     <t>En caso de Docente a Designar</t>
   </si>
   <si>
-    <t>Día</t>
-  </si>
-  <si>
     <t>Edificio</t>
   </si>
   <si>
@@ -401,6 +398,9 @@
   </si>
   <si>
     <t>A confirmar día y hora</t>
+  </si>
+  <si>
+    <t>Dia</t>
   </si>
 </sst>
 </file>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="E10" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,68 +784,68 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
         <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
       </c>
       <c r="L3" s="1">
         <v>0.54166666666666663</v>
@@ -854,10 +854,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="N3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P3">
         <v>25</v>
@@ -865,34 +865,34 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
         <v>27</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" t="s">
-        <v>28</v>
       </c>
       <c r="L4" s="1">
         <v>0.33333333333333331</v>
@@ -901,10 +901,10 @@
         <v>0.5</v>
       </c>
       <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
         <v>29</v>
-      </c>
-      <c r="O4" t="s">
-        <v>30</v>
       </c>
       <c r="P4">
         <v>2</v>
@@ -912,34 +912,34 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
         <v>27</v>
-      </c>
-      <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
       </c>
       <c r="L5" s="1">
         <v>0.75</v>
@@ -948,10 +948,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" t="s">
         <v>29</v>
-      </c>
-      <c r="O5" t="s">
-        <v>30</v>
       </c>
       <c r="P5">
         <v>2</v>
@@ -959,34 +959,34 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
       </c>
       <c r="G6">
         <v>4</v>
       </c>
       <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
         <v>31</v>
-      </c>
-      <c r="J6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" t="s">
-        <v>32</v>
       </c>
       <c r="L6" s="1">
         <v>0.75</v>
@@ -995,10 +995,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" t="s">
         <v>29</v>
-      </c>
-      <c r="O6" t="s">
-        <v>30</v>
       </c>
       <c r="P6">
         <v>2</v>
@@ -1006,34 +1006,34 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
       </c>
       <c r="G7">
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L7" s="1">
         <v>0.33333333333333331</v>
@@ -1042,10 +1042,10 @@
         <v>0.5</v>
       </c>
       <c r="N7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" t="s">
         <v>29</v>
-      </c>
-      <c r="O7" t="s">
-        <v>30</v>
       </c>
       <c r="P7">
         <v>2</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1062,25 +1062,25 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L8" s="1">
         <v>0.75</v>
@@ -1089,10 +1089,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P8">
         <v>120</v>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1109,25 +1109,25 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
         <v>34</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>35</v>
-      </c>
-      <c r="F9" t="s">
-        <v>36</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L9" s="1">
         <v>0.79166666666666663</v>
@@ -1136,10 +1136,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P9">
         <v>25</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1156,25 +1156,25 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
       <c r="G10">
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
         <v>23</v>
-      </c>
-      <c r="K10" t="s">
-        <v>24</v>
       </c>
       <c r="L10" s="1">
         <v>0.33333333333333331</v>
@@ -1183,10 +1183,10 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="N10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P10">
         <v>26</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1203,25 +1203,25 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>35</v>
       </c>
-      <c r="F11" t="s">
-        <v>36</v>
-      </c>
       <c r="G11">
         <v>2</v>
       </c>
       <c r="H11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" t="s">
         <v>39</v>
-      </c>
-      <c r="J11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" t="s">
-        <v>40</v>
       </c>
       <c r="L11" s="1">
         <v>0.33333333333333331</v>
@@ -1230,10 +1230,10 @@
         <v>0.5</v>
       </c>
       <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" t="s">
         <v>29</v>
-      </c>
-      <c r="O11" t="s">
-        <v>30</v>
       </c>
       <c r="P11">
         <v>2</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -1250,25 +1250,25 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>35</v>
-      </c>
-      <c r="F12" t="s">
-        <v>36</v>
       </c>
       <c r="G12">
         <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" t="s">
         <v>23</v>
-      </c>
-      <c r="K12" t="s">
-        <v>24</v>
       </c>
       <c r="L12" s="1">
         <v>0.5</v>
@@ -1277,10 +1277,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="N12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P12">
         <v>26</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1297,25 +1297,25 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>35</v>
-      </c>
-      <c r="F13" t="s">
-        <v>36</v>
       </c>
       <c r="G13">
         <v>3</v>
       </c>
       <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" t="s">
         <v>39</v>
-      </c>
-      <c r="J13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" t="s">
-        <v>40</v>
       </c>
       <c r="L13" s="1">
         <v>0.5</v>
@@ -1324,10 +1324,10 @@
         <v>0.625</v>
       </c>
       <c r="N13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" t="s">
         <v>29</v>
-      </c>
-      <c r="O13" t="s">
-        <v>30</v>
       </c>
       <c r="P13">
         <v>2</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1344,25 +1344,25 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
         <v>34</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>35</v>
-      </c>
-      <c r="F14" t="s">
-        <v>36</v>
       </c>
       <c r="G14">
         <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L14" s="1">
         <v>0.33333333333333331</v>
@@ -1371,18 +1371,18 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="N14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" t="s">
+        <v>25</v>
+      </c>
+      <c r="P14" t="s">
         <v>42</v>
-      </c>
-      <c r="O14" t="s">
-        <v>26</v>
-      </c>
-      <c r="P14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1391,25 +1391,25 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
         <v>34</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>35</v>
-      </c>
-      <c r="F15" t="s">
-        <v>36</v>
       </c>
       <c r="G15">
         <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L15" s="1">
         <v>0.33333333333333331</v>
@@ -1418,10 +1418,10 @@
         <v>0.5</v>
       </c>
       <c r="N15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P15">
         <v>25</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -1438,25 +1438,25 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
         <v>44</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>45</v>
-      </c>
-      <c r="F16" t="s">
-        <v>46</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L16" s="1">
         <v>0.54166666666666663</v>
@@ -1465,10 +1465,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="N16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P16">
         <v>25</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1485,25 +1485,25 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
         <v>44</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>45</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
         <v>46</v>
       </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="H17" t="s">
-        <v>47</v>
-      </c>
       <c r="J17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L17" s="1">
         <v>0.33333333333333331</v>
@@ -1512,10 +1512,10 @@
         <v>0.5</v>
       </c>
       <c r="N17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P17">
         <v>26</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1532,25 +1532,25 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
         <v>44</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>45</v>
-      </c>
-      <c r="F18" t="s">
-        <v>46</v>
       </c>
       <c r="G18">
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L18" s="1">
         <v>0.33333333333333331</v>
@@ -1559,10 +1559,10 @@
         <v>0.5</v>
       </c>
       <c r="N18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P18">
         <v>26</v>
@@ -1570,7 +1570,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1579,25 +1579,25 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
         <v>44</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>45</v>
-      </c>
-      <c r="F19" t="s">
-        <v>46</v>
       </c>
       <c r="G19">
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L19" s="1">
         <v>0.54166666666666663</v>
@@ -1606,10 +1606,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="N19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P19">
         <v>25</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -1626,25 +1626,25 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
         <v>44</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>45</v>
-      </c>
-      <c r="F20" t="s">
-        <v>46</v>
       </c>
       <c r="G20">
         <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L20" s="1">
         <v>0.75</v>
@@ -1653,10 +1653,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P20">
         <v>39</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -1673,25 +1673,25 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
         <v>44</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>45</v>
-      </c>
-      <c r="F21" t="s">
-        <v>46</v>
       </c>
       <c r="G21">
         <v>5</v>
       </c>
       <c r="H21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L21" s="1">
         <v>0.83333333333333337</v>
@@ -1700,10 +1700,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P21">
         <v>26</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -1720,25 +1720,25 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="s">
         <v>51</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>52</v>
-      </c>
-      <c r="F22" t="s">
-        <v>53</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" t="s">
         <v>53</v>
-      </c>
-      <c r="J22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" t="s">
-        <v>54</v>
       </c>
       <c r="L22" s="1">
         <v>0.45833333333333331</v>
@@ -1747,10 +1747,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="N22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P22">
         <v>21</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1767,25 +1767,25 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
         <v>51</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>52</v>
-      </c>
-      <c r="F23" t="s">
-        <v>53</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23" t="s">
+        <v>52</v>
+      </c>
+      <c r="J23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" t="s">
         <v>53</v>
-      </c>
-      <c r="J23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23" t="s">
-        <v>54</v>
       </c>
       <c r="L23" s="1">
         <v>0.54166666666666663</v>
@@ -1794,10 +1794,10 @@
         <v>0.625</v>
       </c>
       <c r="N23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P23">
         <v>25</v>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1814,25 +1814,25 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
         <v>51</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>52</v>
       </c>
-      <c r="F24" t="s">
-        <v>53</v>
-      </c>
       <c r="G24">
         <v>2</v>
       </c>
       <c r="H24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L24" s="1">
         <v>0.33333333333333331</v>
@@ -1841,10 +1841,10 @@
         <v>0.5</v>
       </c>
       <c r="N24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P24">
         <v>25</v>
@@ -1852,7 +1852,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1861,25 +1861,25 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" t="s">
         <v>51</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>52</v>
-      </c>
-      <c r="F25" t="s">
-        <v>53</v>
       </c>
       <c r="G25">
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" t="s">
         <v>23</v>
-      </c>
-      <c r="K25" t="s">
-        <v>24</v>
       </c>
       <c r="L25" s="1">
         <v>0.70833333333333337</v>
@@ -1888,10 +1888,10 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="N25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P25">
         <v>25</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -1908,25 +1908,25 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s">
         <v>51</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>52</v>
-      </c>
-      <c r="F26" t="s">
-        <v>53</v>
       </c>
       <c r="G26">
         <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L26" s="1">
         <v>0.70833333333333337</v>
@@ -1935,10 +1935,10 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="N26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P26">
         <v>25</v>
@@ -1946,7 +1946,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1955,25 +1955,25 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" t="s">
         <v>51</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>52</v>
-      </c>
-      <c r="F27" t="s">
-        <v>53</v>
       </c>
       <c r="G27">
         <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L27" s="1">
         <v>0.54166666666666663</v>
@@ -1982,10 +1982,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="N27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P27">
         <v>25</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -2002,25 +2002,25 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" t="s">
         <v>58</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>59</v>
-      </c>
-      <c r="F28" t="s">
-        <v>60</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L28" s="1">
         <v>0.33333333333333331</v>
@@ -2029,10 +2029,10 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="N28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P28">
         <v>26</v>
@@ -2040,7 +2040,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -2049,25 +2049,25 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" t="s">
         <v>58</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>59</v>
       </c>
-      <c r="F29" t="s">
-        <v>60</v>
-      </c>
       <c r="G29">
         <v>2</v>
       </c>
       <c r="H29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L29" s="1">
         <v>0.79166666666666663</v>
@@ -2076,10 +2076,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P29">
         <v>26</v>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -2096,25 +2096,25 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" t="s">
         <v>61</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>62</v>
-      </c>
-      <c r="F30" t="s">
-        <v>63</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L30" s="1">
         <v>0.33333333333333331</v>
@@ -2123,10 +2123,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="N30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P30">
         <v>26</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -2143,25 +2143,25 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" t="s">
         <v>61</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>62</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31" t="s">
         <v>63</v>
       </c>
-      <c r="G31">
-        <v>2</v>
-      </c>
-      <c r="H31" t="s">
-        <v>64</v>
-      </c>
       <c r="J31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L31" s="1">
         <v>0.33333333333333331</v>
@@ -2170,10 +2170,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="N31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P31">
         <v>25</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -2190,25 +2190,25 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" t="s">
         <v>61</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>62</v>
-      </c>
-      <c r="F32" t="s">
-        <v>63</v>
       </c>
       <c r="G32">
         <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L32" s="1">
         <v>0.33333333333333331</v>
@@ -2217,10 +2217,10 @@
         <v>0.4375</v>
       </c>
       <c r="N32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P32">
         <v>30</v>
@@ -2228,7 +2228,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -2237,25 +2237,25 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" t="s">
         <v>61</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>62</v>
-      </c>
-      <c r="F33" t="s">
-        <v>63</v>
       </c>
       <c r="G33">
         <v>3</v>
       </c>
       <c r="H33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L33" s="1">
         <v>0.4375</v>
@@ -2264,10 +2264,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="N33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P33">
         <v>26</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -2284,25 +2284,25 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" t="s">
         <v>61</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>62</v>
-      </c>
-      <c r="F34" t="s">
-        <v>63</v>
       </c>
       <c r="G34">
         <v>4</v>
       </c>
       <c r="H34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L34" s="1">
         <v>0.79166666666666663</v>
@@ -2311,10 +2311,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P34">
         <v>25</v>
@@ -2322,7 +2322,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -2331,25 +2331,25 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" t="s">
         <v>61</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>62</v>
-      </c>
-      <c r="F35" t="s">
-        <v>63</v>
       </c>
       <c r="G35">
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L35" s="1">
         <v>0.83333333333333337</v>
@@ -2358,10 +2358,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P35">
         <v>26</v>
@@ -2369,7 +2369,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -2378,25 +2378,25 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" t="s">
         <v>66</v>
       </c>
-      <c r="E36" t="s">
-        <v>67</v>
-      </c>
       <c r="F36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L36" s="1">
         <v>0.33333333333333331</v>
@@ -2405,10 +2405,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="N36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P36">
         <v>25</v>
@@ -2416,7 +2416,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -2425,25 +2425,25 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" t="s">
         <v>66</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37" t="s">
         <v>67</v>
       </c>
-      <c r="F37" t="s">
-        <v>21</v>
-      </c>
-      <c r="G37">
-        <v>2</v>
-      </c>
-      <c r="H37" t="s">
-        <v>68</v>
-      </c>
       <c r="J37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L37" s="1">
         <v>0.54166666666666663</v>
@@ -2452,10 +2452,10 @@
         <v>0.75</v>
       </c>
       <c r="N37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P37">
         <v>26</v>
@@ -2463,7 +2463,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -2472,25 +2472,25 @@
         <v>3</v>
       </c>
       <c r="D38" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" t="s">
         <v>66</v>
       </c>
-      <c r="E38" t="s">
-        <v>67</v>
-      </c>
       <c r="F38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G38">
         <v>3</v>
       </c>
       <c r="H38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" t="s">
+        <v>22</v>
+      </c>
+      <c r="K38" t="s">
         <v>27</v>
-      </c>
-      <c r="J38" t="s">
-        <v>23</v>
-      </c>
-      <c r="K38" t="s">
-        <v>28</v>
       </c>
       <c r="L38" s="1">
         <v>0.54166666666666663</v>
@@ -2499,10 +2499,10 @@
         <v>0.75</v>
       </c>
       <c r="N38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P38">
         <v>26</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -2519,25 +2519,25 @@
         <v>3</v>
       </c>
       <c r="D39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" t="s">
         <v>69</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>70</v>
-      </c>
-      <c r="F39" t="s">
-        <v>71</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L39" s="1">
         <v>0.5</v>
@@ -2546,10 +2546,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="N39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P39">
         <v>26</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -2566,25 +2566,25 @@
         <v>3</v>
       </c>
       <c r="D40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" t="s">
         <v>69</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>70</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40" t="s">
         <v>71</v>
       </c>
-      <c r="G40">
-        <v>2</v>
-      </c>
-      <c r="H40" t="s">
-        <v>72</v>
-      </c>
       <c r="J40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L40" s="1">
         <v>0.41666666666666669</v>
@@ -2593,10 +2593,10 @@
         <v>0.625</v>
       </c>
       <c r="N40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P40">
         <v>32</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -2613,25 +2613,25 @@
         <v>3</v>
       </c>
       <c r="D41" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" t="s">
         <v>73</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>74</v>
-      </c>
-      <c r="F41" t="s">
-        <v>75</v>
       </c>
       <c r="G41">
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J41" t="s">
+        <v>22</v>
+      </c>
+      <c r="K41" t="s">
         <v>23</v>
-      </c>
-      <c r="K41" t="s">
-        <v>24</v>
       </c>
       <c r="L41" s="1">
         <v>0.33333333333333331</v>
@@ -2640,10 +2640,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="N41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P41">
         <v>25</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -2660,25 +2660,25 @@
         <v>3</v>
       </c>
       <c r="D42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" t="s">
         <v>76</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>77</v>
-      </c>
-      <c r="F42" t="s">
-        <v>78</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L42" s="1">
         <v>0.70833333333333337</v>
@@ -2687,10 +2687,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P42">
         <v>26</v>
@@ -2698,7 +2698,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -2707,25 +2707,25 @@
         <v>3</v>
       </c>
       <c r="D43" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" t="s">
         <v>80</v>
       </c>
-      <c r="E43" t="s">
-        <v>81</v>
-      </c>
       <c r="F43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J43" t="s">
+        <v>22</v>
+      </c>
+      <c r="K43" t="s">
         <v>23</v>
-      </c>
-      <c r="K43" t="s">
-        <v>24</v>
       </c>
       <c r="L43" s="1">
         <v>0.625</v>
@@ -2734,10 +2734,10 @@
         <v>0.75</v>
       </c>
       <c r="N43" t="s">
+        <v>28</v>
+      </c>
+      <c r="O43" t="s">
         <v>29</v>
-      </c>
-      <c r="O43" t="s">
-        <v>30</v>
       </c>
       <c r="P43">
         <v>2</v>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -2754,25 +2754,25 @@
         <v>3</v>
       </c>
       <c r="D44" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" t="s">
         <v>80</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44" t="s">
         <v>81</v>
       </c>
-      <c r="F44" t="s">
-        <v>75</v>
-      </c>
-      <c r="G44">
-        <v>2</v>
-      </c>
-      <c r="H44" t="s">
-        <v>82</v>
-      </c>
       <c r="J44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L44" s="1">
         <v>0.625</v>
@@ -2781,10 +2781,10 @@
         <v>0.75</v>
       </c>
       <c r="N44" t="s">
+        <v>28</v>
+      </c>
+      <c r="O44" t="s">
         <v>29</v>
-      </c>
-      <c r="O44" t="s">
-        <v>30</v>
       </c>
       <c r="P44">
         <v>2</v>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -2801,25 +2801,25 @@
         <v>3</v>
       </c>
       <c r="D45" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" t="s">
         <v>80</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45" t="s">
         <v>81</v>
       </c>
-      <c r="F45" t="s">
-        <v>75</v>
-      </c>
-      <c r="G45">
-        <v>2</v>
-      </c>
-      <c r="H45" t="s">
-        <v>82</v>
-      </c>
       <c r="J45" t="s">
+        <v>22</v>
+      </c>
+      <c r="K45" t="s">
         <v>23</v>
-      </c>
-      <c r="K45" t="s">
-        <v>24</v>
       </c>
       <c r="L45" s="1">
         <v>0.83333333333333337</v>
@@ -2828,10 +2828,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N45" t="s">
+        <v>28</v>
+      </c>
+      <c r="O45" t="s">
         <v>29</v>
-      </c>
-      <c r="O45" t="s">
-        <v>30</v>
       </c>
       <c r="P45">
         <v>2</v>
@@ -2839,7 +2839,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -2848,25 +2848,25 @@
         <v>3</v>
       </c>
       <c r="D46" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" t="s">
         <v>80</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
+        <v>74</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46" t="s">
         <v>81</v>
       </c>
-      <c r="F46" t="s">
-        <v>75</v>
-      </c>
-      <c r="G46">
-        <v>2</v>
-      </c>
-      <c r="H46" t="s">
-        <v>82</v>
-      </c>
       <c r="J46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L46" s="1">
         <v>0.75</v>
@@ -2875,10 +2875,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N46" t="s">
+        <v>28</v>
+      </c>
+      <c r="O46" t="s">
         <v>29</v>
-      </c>
-      <c r="O46" t="s">
-        <v>30</v>
       </c>
       <c r="P46">
         <v>2</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -2895,25 +2895,25 @@
         <v>3</v>
       </c>
       <c r="D47" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" t="s">
         <v>83</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>84</v>
-      </c>
-      <c r="F47" t="s">
-        <v>85</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J47" t="s">
+        <v>22</v>
+      </c>
+      <c r="K47" t="s">
         <v>23</v>
-      </c>
-      <c r="K47" t="s">
-        <v>24</v>
       </c>
       <c r="L47" s="1">
         <v>0.70833333333333337</v>
@@ -2922,10 +2922,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P47">
         <v>26</v>
@@ -2933,7 +2933,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -2942,25 +2942,25 @@
         <v>3</v>
       </c>
       <c r="D48" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" t="s">
         <v>83</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>84</v>
-      </c>
-      <c r="F48" t="s">
-        <v>85</v>
       </c>
       <c r="G48">
         <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L48" s="1">
         <v>0.70833333333333337</v>
@@ -2969,10 +2969,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P48">
         <v>27</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -2989,25 +2989,25 @@
         <v>3</v>
       </c>
       <c r="D49" t="s">
+        <v>85</v>
+      </c>
+      <c r="E49" t="s">
         <v>86</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>87</v>
-      </c>
-      <c r="F49" t="s">
-        <v>88</v>
       </c>
       <c r="G49">
         <v>1</v>
       </c>
       <c r="H49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L49" s="1">
         <v>0.75</v>
@@ -3016,10 +3016,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P49">
         <v>414</v>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -3036,22 +3036,22 @@
         <v>3</v>
       </c>
       <c r="D50" t="s">
+        <v>85</v>
+      </c>
+      <c r="E50" t="s">
         <v>86</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>87</v>
       </c>
-      <c r="F50" t="s">
-        <v>88</v>
-      </c>
       <c r="G50">
         <v>2</v>
       </c>
       <c r="J50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L50" s="1">
         <v>0.33333333333333331</v>
@@ -3060,10 +3060,10 @@
         <v>0.5</v>
       </c>
       <c r="N50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P50">
         <v>24</v>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -3080,25 +3080,25 @@
         <v>4</v>
       </c>
       <c r="D51" t="s">
+        <v>89</v>
+      </c>
+      <c r="E51" t="s">
         <v>90</v>
       </c>
-      <c r="E51" t="s">
-        <v>91</v>
-      </c>
       <c r="F51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G51">
         <v>1</v>
       </c>
       <c r="H51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J51" t="s">
+        <v>22</v>
+      </c>
+      <c r="K51" t="s">
         <v>23</v>
-      </c>
-      <c r="K51" t="s">
-        <v>24</v>
       </c>
       <c r="L51" s="1">
         <v>0.79166666666666663</v>
@@ -3107,10 +3107,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P51">
         <v>25</v>
@@ -3118,7 +3118,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B52">
         <v>2</v>
@@ -3127,25 +3127,25 @@
         <v>4</v>
       </c>
       <c r="D52" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" t="s">
         <v>90</v>
       </c>
-      <c r="E52" t="s">
-        <v>91</v>
-      </c>
       <c r="F52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G52">
         <v>1</v>
       </c>
       <c r="H52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L52" s="1">
         <v>0.79166666666666663</v>
@@ -3154,18 +3154,18 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -3174,25 +3174,25 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" t="s">
         <v>93</v>
       </c>
-      <c r="E53" t="s">
-        <v>94</v>
-      </c>
       <c r="F53" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G53">
         <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L53" s="1">
         <v>0.33333333333333331</v>
@@ -3201,10 +3201,10 @@
         <v>0.4375</v>
       </c>
       <c r="N53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P53">
         <v>26</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -3221,25 +3221,25 @@
         <v>4</v>
       </c>
       <c r="D54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54" t="s">
         <v>93</v>
       </c>
-      <c r="E54" t="s">
-        <v>94</v>
-      </c>
       <c r="F54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G54">
         <v>1</v>
       </c>
       <c r="H54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L54" s="1">
         <v>0.4375</v>
@@ -3248,10 +3248,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="N54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P54">
         <v>30</v>
@@ -3259,7 +3259,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -3268,25 +3268,25 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
+        <v>92</v>
+      </c>
+      <c r="E55" t="s">
         <v>93</v>
       </c>
-      <c r="E55" t="s">
-        <v>94</v>
-      </c>
       <c r="F55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G55">
         <v>2</v>
       </c>
       <c r="H55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L55" s="1">
         <v>0.5</v>
@@ -3295,10 +3295,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="N55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P55">
         <v>25</v>
@@ -3306,7 +3306,7 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B56">
         <v>2</v>
@@ -3315,25 +3315,25 @@
         <v>4</v>
       </c>
       <c r="D56" t="s">
+        <v>95</v>
+      </c>
+      <c r="E56" t="s">
         <v>96</v>
       </c>
-      <c r="E56" t="s">
-        <v>97</v>
-      </c>
       <c r="F56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G56">
         <v>1</v>
       </c>
       <c r="H56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L56" s="1">
         <v>0.75</v>
@@ -3342,10 +3342,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P56">
         <v>62</v>
@@ -3353,7 +3353,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -3362,25 +3362,25 @@
         <v>4</v>
       </c>
       <c r="D57" t="s">
+        <v>98</v>
+      </c>
+      <c r="E57" t="s">
         <v>99</v>
       </c>
-      <c r="E57" t="s">
-        <v>100</v>
-      </c>
       <c r="F57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J57" t="s">
+        <v>22</v>
+      </c>
+      <c r="K57" t="s">
         <v>23</v>
-      </c>
-      <c r="K57" t="s">
-        <v>24</v>
       </c>
       <c r="L57" s="1">
         <v>0.79166666666666663</v>
@@ -3389,10 +3389,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P57">
         <v>307</v>
@@ -3400,7 +3400,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -3409,25 +3409,25 @@
         <v>4</v>
       </c>
       <c r="D58" t="s">
+        <v>98</v>
+      </c>
+      <c r="E58" t="s">
         <v>99</v>
       </c>
-      <c r="E58" t="s">
-        <v>100</v>
-      </c>
       <c r="F58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G58">
         <v>1</v>
       </c>
       <c r="H58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L58" s="1">
         <v>0.79166666666666663</v>
@@ -3436,10 +3436,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P58">
         <v>25</v>
@@ -3447,7 +3447,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -3456,25 +3456,25 @@
         <v>4</v>
       </c>
       <c r="D59" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" t="s">
         <v>101</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>102</v>
-      </c>
-      <c r="F59" t="s">
-        <v>103</v>
       </c>
       <c r="G59">
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L59" s="1">
         <v>0.70833333333333337</v>
@@ -3483,10 +3483,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O59" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P59">
         <v>305</v>
@@ -3494,7 +3494,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B60">
         <v>2</v>
@@ -3503,25 +3503,25 @@
         <v>4</v>
       </c>
       <c r="D60" t="s">
+        <v>103</v>
+      </c>
+      <c r="E60" t="s">
         <v>104</v>
       </c>
-      <c r="E60" t="s">
-        <v>105</v>
-      </c>
       <c r="F60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G60">
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K60" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L60" s="1">
         <v>0.70833333333333337</v>
@@ -3530,10 +3530,10 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="N60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P60">
         <v>25</v>
@@ -3541,7 +3541,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -3550,25 +3550,25 @@
         <v>4</v>
       </c>
       <c r="D61" t="s">
+        <v>103</v>
+      </c>
+      <c r="E61" t="s">
         <v>104</v>
       </c>
-      <c r="E61" t="s">
-        <v>105</v>
-      </c>
       <c r="F61" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G61">
         <v>1</v>
       </c>
       <c r="H61" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L61" s="1">
         <v>0.79166666666666663</v>
@@ -3577,10 +3577,10 @@
         <v>0.875</v>
       </c>
       <c r="N61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O61" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P61">
         <v>30</v>
@@ -3588,7 +3588,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B62">
         <v>2</v>
@@ -3597,25 +3597,25 @@
         <v>4</v>
       </c>
       <c r="D62" t="s">
+        <v>103</v>
+      </c>
+      <c r="E62" t="s">
         <v>104</v>
       </c>
-      <c r="E62" t="s">
-        <v>105</v>
-      </c>
       <c r="F62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G62">
         <v>1</v>
       </c>
       <c r="H62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J62" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L62" s="1">
         <v>0.70833333333333337</v>
@@ -3624,10 +3624,10 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="N62" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O62" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P62">
         <v>25</v>
@@ -3635,7 +3635,7 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B63">
         <v>2</v>
@@ -3644,25 +3644,25 @@
         <v>4</v>
       </c>
       <c r="D63" t="s">
+        <v>105</v>
+      </c>
+      <c r="E63" t="s">
         <v>106</v>
       </c>
-      <c r="E63" t="s">
-        <v>107</v>
-      </c>
       <c r="F63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G63">
         <v>1</v>
       </c>
       <c r="H63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L63" s="1">
         <v>0.5</v>
@@ -3671,10 +3671,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="N63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P63">
         <v>34</v>
@@ -3682,7 +3682,7 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B64">
         <v>2</v>
@@ -3691,25 +3691,25 @@
         <v>4</v>
       </c>
       <c r="D64" t="s">
+        <v>105</v>
+      </c>
+      <c r="E64" t="s">
         <v>106</v>
       </c>
-      <c r="E64" t="s">
-        <v>107</v>
-      </c>
       <c r="F64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G64">
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L64" s="1">
         <v>0.54166666666666663</v>
@@ -3718,10 +3718,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="N64" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O64" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P64">
         <v>26</v>
@@ -3729,7 +3729,7 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -3738,25 +3738,25 @@
         <v>4</v>
       </c>
       <c r="D65" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" t="s">
         <v>108</v>
       </c>
-      <c r="E65" t="s">
-        <v>109</v>
-      </c>
       <c r="F65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G65">
         <v>1</v>
       </c>
       <c r="H65" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J65" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L65" s="1">
         <v>0.75</v>
@@ -3765,10 +3765,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N65" t="s">
+        <v>28</v>
+      </c>
+      <c r="O65" t="s">
         <v>29</v>
-      </c>
-      <c r="O65" t="s">
-        <v>30</v>
       </c>
       <c r="P65">
         <v>2</v>
@@ -3776,7 +3776,7 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B66">
         <v>2</v>
@@ -3785,25 +3785,25 @@
         <v>5</v>
       </c>
       <c r="D66" t="s">
+        <v>110</v>
+      </c>
+      <c r="E66" t="s">
         <v>111</v>
       </c>
-      <c r="E66" t="s">
-        <v>112</v>
-      </c>
       <c r="F66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G66">
         <v>1</v>
       </c>
       <c r="H66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J66" t="s">
+        <v>22</v>
+      </c>
+      <c r="K66" t="s">
         <v>23</v>
-      </c>
-      <c r="K66" t="s">
-        <v>24</v>
       </c>
       <c r="L66" s="1">
         <v>0.75</v>
@@ -3812,10 +3812,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P66">
         <v>206</v>
@@ -3829,25 +3829,25 @@
         <v>5</v>
       </c>
       <c r="D67" t="s">
+        <v>113</v>
+      </c>
+      <c r="E67" t="s">
         <v>114</v>
       </c>
-      <c r="E67" t="s">
-        <v>115</v>
-      </c>
       <c r="F67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G67">
         <v>1</v>
       </c>
       <c r="H67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K67" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L67" s="1">
         <v>0.75</v>
@@ -3856,10 +3856,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N67" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O67" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P67">
         <v>408</v>
@@ -3873,25 +3873,25 @@
         <v>5</v>
       </c>
       <c r="D68" t="s">
+        <v>113</v>
+      </c>
+      <c r="E68" t="s">
         <v>114</v>
       </c>
-      <c r="E68" t="s">
-        <v>115</v>
-      </c>
       <c r="F68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G68">
         <v>1</v>
       </c>
       <c r="H68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L68" s="1">
         <v>0.83333333333333337</v>
@@ -3900,10 +3900,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N68" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O68" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P68">
         <v>27</v>
@@ -3917,25 +3917,25 @@
         <v>5</v>
       </c>
       <c r="D69" t="s">
+        <v>116</v>
+      </c>
+      <c r="E69" t="s">
         <v>117</v>
       </c>
-      <c r="E69" t="s">
-        <v>118</v>
-      </c>
       <c r="F69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G69">
         <v>1</v>
       </c>
       <c r="H69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J69" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L69" s="1">
         <v>0.33333333333333331</v>
@@ -3944,10 +3944,10 @@
         <v>0.5</v>
       </c>
       <c r="N69" t="s">
+        <v>28</v>
+      </c>
+      <c r="O69" t="s">
         <v>29</v>
-      </c>
-      <c r="O69" t="s">
-        <v>30</v>
       </c>
       <c r="P69">
         <v>2</v>
@@ -3961,25 +3961,25 @@
         <v>5</v>
       </c>
       <c r="D70" t="s">
+        <v>119</v>
+      </c>
+      <c r="E70" t="s">
         <v>120</v>
       </c>
-      <c r="E70" t="s">
-        <v>121</v>
-      </c>
       <c r="F70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G70">
         <v>1</v>
       </c>
       <c r="H70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J70" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K70" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L70" s="1">
         <v>0.54166666666666663</v>
@@ -3988,10 +3988,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="N70" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O70" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P70">
         <v>219</v>
@@ -4005,25 +4005,25 @@
         <v>5</v>
       </c>
       <c r="D71" t="s">
+        <v>121</v>
+      </c>
+      <c r="E71" t="s">
         <v>122</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>123</v>
-      </c>
-      <c r="F71" t="s">
-        <v>124</v>
       </c>
       <c r="G71">
         <v>1</v>
       </c>
       <c r="H71" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J71" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L71" s="1">
         <v>0.70833333333333337</v>
@@ -4032,10 +4032,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="N71" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P71">
         <v>414</v>
@@ -4049,22 +4049,22 @@
         <v>2</v>
       </c>
       <c r="D72" t="s">
+        <v>33</v>
+      </c>
+      <c r="E72" t="s">
         <v>34</v>
       </c>
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>35</v>
       </c>
-      <c r="F72" t="s">
-        <v>36</v>
-      </c>
       <c r="G72" t="s">
+        <v>126</v>
+      </c>
+      <c r="H72" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q72" t="s">
         <v>127</v>
-      </c>
-      <c r="H72" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q72" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -4075,28 +4075,28 @@
         <v>4</v>
       </c>
       <c r="D73" t="s">
+        <v>92</v>
+      </c>
+      <c r="E73" t="s">
         <v>93</v>
       </c>
-      <c r="E73" t="s">
-        <v>94</v>
-      </c>
       <c r="F73" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G73" t="s">
+        <v>126</v>
+      </c>
+      <c r="H73" t="s">
+        <v>40</v>
+      </c>
+      <c r="J73" t="s">
+        <v>22</v>
+      </c>
+      <c r="O73" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q73" t="s">
         <v>127</v>
-      </c>
-      <c r="H73" t="s">
-        <v>41</v>
-      </c>
-      <c r="J73" t="s">
-        <v>23</v>
-      </c>
-      <c r="O73" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>